<commit_message>
data and mppt compare
</commit_message>
<xml_diff>
--- a/spreadsheets/CostBreakdown.xlsx
+++ b/spreadsheets/CostBreakdown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\achen\Dropbox\code\Stability-Setup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\achen\Dropbox\code\Stability-Setup\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E8D4CE-EB4A-45D9-A051-9E59EA2698EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03A0C6E-2086-4067-B4FD-E04DC7A49732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
   <si>
     <t>product</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>number</t>
-  </si>
-  <si>
-    <t>arduino mega</t>
   </si>
   <si>
     <t>arduino due</t>
@@ -440,27 +437,27 @@
   <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,7 +469,7 @@
       </c>
       <c r="D1" s="2">
         <f>SUM(D2:D48)</f>
-        <v>750</v>
+        <v>740</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
@@ -517,22 +514,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2">
         <f t="shared" ref="D2:D8" si="0">B2*C2</f>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G2" s="2">
         <v>50</v>
@@ -545,7 +542,7 @@
         <v>50</v>
       </c>
       <c r="K2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L2" s="2">
         <v>25</v>
@@ -558,7 +555,7 @@
         <v>25</v>
       </c>
       <c r="P2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q2" s="2">
         <v>25</v>
@@ -571,9 +568,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2">
         <v>10</v>
@@ -586,7 +583,7 @@
         <v>320</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3" s="2">
         <v>60</v>
@@ -599,7 +596,7 @@
         <v>480</v>
       </c>
       <c r="K3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L3" s="2">
         <v>10</v>
@@ -612,7 +609,7 @@
         <v>80</v>
       </c>
       <c r="P3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q3" s="2">
         <v>10</v>
@@ -625,9 +622,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2">
         <v>5</v>
@@ -640,7 +637,7 @@
         <v>160</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" s="2">
         <v>10</v>
@@ -653,7 +650,7 @@
         <v>80</v>
       </c>
       <c r="K4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L4" s="2">
         <v>5</v>
@@ -666,7 +663,7 @@
         <v>40</v>
       </c>
       <c r="P4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q4" s="2">
         <v>5</v>
@@ -679,9 +676,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2">
         <v>100</v>
@@ -694,7 +691,7 @@
         <v>100</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5" s="2">
         <v>40</v>
@@ -707,7 +704,7 @@
         <v>40</v>
       </c>
       <c r="K5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L5" s="2">
         <v>50</v>
@@ -720,7 +717,7 @@
         <v>50</v>
       </c>
       <c r="P5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q5" s="2">
         <v>50</v>
@@ -733,9 +730,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1">
         <v>10</v>
@@ -760,9 +757,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1">
         <v>10</v>
@@ -787,9 +784,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1">
         <v>30</v>

</xml_diff>